<commit_message>
improve the code to generate expectResult, edit in XGDQA006 vm
</commit_message>
<xml_diff>
--- a/template_RGpath.xlsx
+++ b/template_RGpath.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBD9D5B-2643-4052-85FB-E85F846021E6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A123676C-90D2-4FBA-AD90-7587B8A2D85E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7515,11 +7515,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7527,17 +7527,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7856,45 +7856,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="65" t="s">
+      <c r="D1" s="70"/>
+      <c r="E1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="66"/>
-      <c r="G1" s="65" t="s">
+      <c r="F1" s="70"/>
+      <c r="G1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="66"/>
-      <c r="I1" s="65" t="s">
+      <c r="H1" s="70"/>
+      <c r="I1" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="66"/>
-      <c r="K1" s="65" t="s">
+      <c r="J1" s="70"/>
+      <c r="K1" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="66"/>
-      <c r="M1" s="65" t="s">
+      <c r="L1" s="70"/>
+      <c r="M1" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="66"/>
+      <c r="N1" s="70"/>
       <c r="O1" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="69" t="s">
+      <c r="P1" s="71" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
+      <c r="A2" s="66"/>
       <c r="B2" s="68"/>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -7933,7 +7933,7 @@
         <v>11</v>
       </c>
       <c r="O2" s="68"/>
-      <c r="P2" s="70"/>
+      <c r="P2" s="72"/>
     </row>
     <row r="3" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -25100,16 +25100,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25146,53 +25146,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="65" t="s">
+      <c r="D1" s="70"/>
+      <c r="E1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="66"/>
-      <c r="G1" s="65" t="s">
+      <c r="F1" s="70"/>
+      <c r="G1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="66"/>
-      <c r="I1" s="65" t="s">
+      <c r="H1" s="70"/>
+      <c r="I1" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="66"/>
-      <c r="K1" s="65" t="s">
+      <c r="J1" s="70"/>
+      <c r="K1" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="66"/>
-      <c r="M1" s="65" t="s">
+      <c r="L1" s="70"/>
+      <c r="M1" s="69" t="s">
         <v>2051</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="65" t="s">
+      <c r="N1" s="70"/>
+      <c r="O1" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="65" t="s">
+      <c r="P1" s="70"/>
+      <c r="Q1" s="69" t="s">
         <v>2052</v>
       </c>
-      <c r="R1" s="66"/>
+      <c r="R1" s="70"/>
       <c r="S1" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="69" t="s">
+      <c r="T1" s="71" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
+      <c r="A2" s="66"/>
       <c r="B2" s="68"/>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -25243,7 +25243,7 @@
         <v>11</v>
       </c>
       <c r="S2" s="68"/>
-      <c r="T2" s="70"/>
+      <c r="T2" s="72"/>
     </row>
     <row r="3" spans="1:20" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -46215,10 +46215,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="77" t="s">
@@ -46229,7 +46229,7 @@
         <v>510</v>
       </c>
       <c r="F1" s="78"/>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="71" t="s">
         <v>511</v>
       </c>
       <c r="H1" s="74" t="s">
@@ -72197,8 +72197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D068D20E-DF69-4AF8-A36A-ACC708DDF8FB}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72209,436 +72209,436 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2120</v>
+        <v>2066</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2154</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2119</v>
+        <v>2065</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2153</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2118</v>
+        <v>1038</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2138</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2117</v>
+        <v>2099</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2140</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2112</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2113</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2114</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2115</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2116</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>2058</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
         <v>2124</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="64" t="s">
         <v>2122</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B15" t="s">
         <v>2125</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="63" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="63" t="s">
         <v>2123</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B16" t="s">
         <v>2156</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="63" t="s">
         <v>2077</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B17" t="s">
         <v>2126</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="63" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="63" t="s">
         <v>2078</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B18" t="s">
         <v>2127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2068</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2053</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2073</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>2061</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2141</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2062</v>
+        <v>2068</v>
       </c>
       <c r="B19" t="s">
-        <v>2126</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2072</v>
+        <v>2053</v>
       </c>
       <c r="B20" t="s">
-        <v>2136</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="B21" t="s">
-        <v>2130</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2067</v>
+        <v>2061</v>
       </c>
       <c r="B22" t="s">
-        <v>2137</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2100</v>
+        <v>2062</v>
       </c>
       <c r="B23" t="s">
-        <v>2131</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2054</v>
+        <v>2072</v>
       </c>
       <c r="B24" t="s">
-        <v>2129</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>2074</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2130</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
       <c r="B26" t="s">
-        <v>2133</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>2055</v>
+        <v>2100</v>
       </c>
       <c r="B27" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>2060</v>
+        <v>2054</v>
       </c>
       <c r="B28" t="s">
-        <v>2138</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2071</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2139</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1038</v>
+        <v>2069</v>
       </c>
       <c r="B30" t="s">
-        <v>2138</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2099</v>
+        <v>2055</v>
       </c>
       <c r="B31" t="s">
-        <v>2140</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>2076</v>
+        <v>2060</v>
       </c>
       <c r="B32" t="s">
-        <v>2134</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>2080</v>
+        <v>2071</v>
       </c>
       <c r="B33" t="s">
-        <v>2158</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>2081</v>
+        <v>2076</v>
       </c>
       <c r="B34" t="s">
-        <v>2159</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>2082</v>
+        <v>2080</v>
       </c>
       <c r="B35" t="s">
-        <v>2160</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
       <c r="B36" t="s">
-        <v>2161</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
       <c r="B37" t="s">
-        <v>2162</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>2085</v>
+        <v>2083</v>
       </c>
       <c r="B38" t="s">
-        <v>2163</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>2086</v>
+        <v>2084</v>
       </c>
       <c r="B39" t="s">
-        <v>2164</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>2087</v>
+        <v>2085</v>
       </c>
       <c r="B40" t="s">
-        <v>2165</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>2088</v>
+        <v>2086</v>
       </c>
       <c r="B41" t="s">
-        <v>2166</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
       <c r="B42" t="s">
-        <v>2167</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>2090</v>
+        <v>2088</v>
       </c>
       <c r="B43" t="s">
-        <v>2168</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>2091</v>
+        <v>2089</v>
       </c>
       <c r="B44" t="s">
-        <v>2169</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="B45" t="s">
-        <v>2170</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B46" t="s">
-        <v>2171</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>2094</v>
+        <v>2092</v>
       </c>
       <c r="B47" t="s">
-        <v>2172</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>2095</v>
+        <v>2093</v>
       </c>
       <c r="B48" t="s">
-        <v>2173</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
       <c r="B49" t="s">
-        <v>2175</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>2097</v>
+        <v>2095</v>
       </c>
       <c r="B50" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>2098</v>
+        <v>2096</v>
       </c>
       <c r="B51" t="s">
-        <v>2157</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>2079</v>
+        <v>2097</v>
       </c>
       <c r="B52" t="s">
-        <v>2150</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>2102</v>
+        <v>2098</v>
       </c>
       <c r="B53" t="s">
-        <v>2142</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>2063</v>
+        <v>2079</v>
       </c>
       <c r="B54" t="s">
-        <v>2127</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>2064</v>
+        <v>2102</v>
       </c>
       <c r="B55" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>2059</v>
+        <v>2063</v>
       </c>
       <c r="B56" t="s">
-        <v>2144</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>2066</v>
+        <v>2064</v>
       </c>
       <c r="B57" t="s">
-        <v>2154</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>2065</v>
+        <v>2059</v>
       </c>
       <c r="B58" t="s">
-        <v>2153</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -72714,8 +72714,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B65">
-    <sortCondition ref="A1"/>
+  <sortState ref="A5:B65">
+    <sortCondition ref="A5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>